<commit_message>
update clinical_notes file, scrapped data
</commit_message>
<xml_diff>
--- a/output/clinical_files/Ovarian Bevacizumab Response/Final patient_list.xlsx
+++ b/output/clinical_files/Ovarian Bevacizumab Response/Final patient_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/honomichlnatasha/Documents/pathology/OvarianBevacizumabResponse_Taiwan/new_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/george/fed/actcianable/output/clinical_files/Ovarian Bevacizumab Response/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39A05C8-1EB9-B74F-8F2E-663488162BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B1246F-CD76-0741-8501-F1027AA240E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20940" yWindow="2980" windowWidth="29080" windowHeight="21460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41040" yWindow="2500" windowWidth="29080" windowHeight="20380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="prob" sheetId="2" r:id="rId1"/>
@@ -695,11 +695,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF81"/>
+  <dimension ref="A1:Q81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I3" sqref="I3"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -721,7 +721,7 @@
     <col min="16" max="16" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>55</v>
       </c>
@@ -766,11 +766,8 @@
       </c>
       <c r="P1" s="10"/>
       <c r="Q1" s="10"/>
-      <c r="AF1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="J2" s="6"/>
       <c r="K2" s="8"/>
@@ -779,7 +776,7 @@
       <c r="N2" s="6"/>
       <c r="P2"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -827,7 +824,7 @@
       </c>
       <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -875,7 +872,7 @@
       </c>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -923,7 +920,7 @@
       </c>
       <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -971,7 +968,7 @@
       </c>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -1019,7 +1016,7 @@
       </c>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1067,7 +1064,7 @@
       </c>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -1115,7 +1112,7 @@
       </c>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1163,7 +1160,7 @@
       </c>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1211,7 +1208,7 @@
       </c>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1259,7 +1256,7 @@
       </c>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1307,7 +1304,7 @@
       </c>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1355,7 +1352,7 @@
       </c>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1403,7 +1400,7 @@
       </c>
       <c r="Q15" s="5"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>14</v>
       </c>

</xml_diff>